<commit_message>
Actividades 6, 7 y 8
Hay un error porque me parece que me toma el df completo y no la base "respondieron" para los cálculos finales. Por favor revisen.
</commit_message>
<xml_diff>
--- a/TP1/datos/tabla_adulto_equiv.xlsx
+++ b/TP1/datos/tabla_adulto_equiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pupih\Desktop\EPH_usu_1_Trim_2019_xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6964f403329964a4/Documents/GitHub/BigDataUBA-GrupoJLP/TP1/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E962F3C-29E4-4745-A82B-33515FD15C1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{6E962F3C-29E4-4745-A82B-33515FD15C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A684BFA-11BB-4E07-B9F8-84966C3B28FB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla de adulo equivalente" sheetId="7" r:id="rId1"/>
@@ -20,7 +20,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -150,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -273,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -301,7 +306,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -312,7 +317,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -321,6 +326,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,9 +345,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -379,9 +385,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,26 +420,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -466,26 +455,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -658,14 +630,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -1007,7 +979,10 @@
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
-      <c r="E33" s="14"/>
+      <c r="E33" s="19">
+        <f>+B25+C24+B27</f>
+        <v>2.46</v>
+      </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>

</xml_diff>